<commit_message>
Use latest DDL files with updated table and column names
</commit_message>
<xml_diff>
--- a/database/SDC CDM Requirements.xlsx
+++ b/database/SDC CDM Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thecap-my.sharepoint.com/personal/agoel_cap_org/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghavan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D56AFB9B-1A89-453A-A044-85D54FFC56A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776214D8-9724-0144-A143-3DB2AAB18C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="878" yWindow="1005" windowWidth="27540" windowHeight="15083" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="32000" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="SdcObs" sheetId="1" r:id="rId1"/>
@@ -79,253 +79,247 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
-  <si>
-    <t>SdcObsClass</t>
-  </si>
-  <si>
-    <t>TemplateInstanceClass (DiagReport)</t>
-  </si>
-  <si>
-    <t>TemplateSdcClass</t>
-  </si>
-  <si>
-    <t>TemplateTermMapClass</t>
-  </si>
-  <si>
-    <t>TemplateMapContentClass</t>
-  </si>
-  <si>
-    <t>PK</t>
-  </si>
-  <si>
-    <t>TemplateInstanceClassFK</t>
-  </si>
-  <si>
-    <t>TemplateInstanceVersionGuid</t>
-  </si>
-  <si>
-    <t>SDCFormDesignID (FD or Pkg)</t>
-  </si>
-  <si>
-    <t>TemplateMapID</t>
-  </si>
-  <si>
-    <t>TemplateTermMap_FK</t>
-  </si>
-  <si>
-    <t>ParentFK</t>
-  </si>
-  <si>
-    <t>TemplateInstanceVersionURI</t>
-  </si>
-  <si>
-    <t>BaseURI</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>TargetID</t>
-  </si>
-  <si>
-    <t>ParentInstanceGuid</t>
-  </si>
-  <si>
-    <t>TemplateSdcFK</t>
-  </si>
-  <si>
-    <t>Lineage</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>InstanceVersionDate</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>MapXML</t>
-  </si>
-  <si>
-    <t>CodeText</t>
-  </si>
-  <si>
-    <t>Section_ID</t>
-  </si>
-  <si>
-    <t>DiagReportProps…</t>
-  </si>
-  <si>
-    <t>FullURI</t>
-  </si>
-  <si>
-    <t>CodeSystemName</t>
-  </si>
-  <si>
-    <t>CodeMatch</t>
-  </si>
-  <si>
-    <t>Section_Guid</t>
-  </si>
-  <si>
-    <t>FormTitle</t>
-  </si>
-  <si>
-    <t>CodeSystemReleaseDate</t>
-  </si>
-  <si>
-    <t>SurgPathID</t>
-  </si>
-  <si>
-    <t>SDC_XML</t>
-  </si>
-  <si>
-    <t>CodeSystemVersion</t>
-  </si>
-  <si>
-    <t>Q_Text</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
   <si>
     <t>(other IDs etc.)</t>
   </si>
   <si>
-    <t>DocType (FD or Pkg)</t>
-  </si>
-  <si>
-    <t>CodeSystemOID</t>
-  </si>
-  <si>
-    <t>Q_InstanceGuid</t>
-  </si>
-  <si>
-    <t>PersonFK</t>
-  </si>
-  <si>
-    <t>CodeSystemURI</t>
-  </si>
-  <si>
-    <t>Q_ID</t>
-  </si>
-  <si>
-    <t>EncounterFK</t>
-  </si>
-  <si>
-    <t>LI_Text</t>
-  </si>
-  <si>
-    <t>PractitionerFK</t>
-  </si>
-  <si>
-    <t>LI_ID</t>
-  </si>
-  <si>
-    <t>LI_InstanceGuid</t>
-  </si>
-  <si>
-    <t>ReportText</t>
-  </si>
-  <si>
     <t>Columns D to F above are data dictionary tables</t>
   </si>
   <si>
-    <t>LI_ParentGuid ?</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>ObservationSpecimensClass</t>
-  </si>
-  <si>
-    <t>SpecimenClass</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>ObservationSpecimensClassPK</t>
-  </si>
-  <si>
-    <t>SpecimenPK</t>
-  </si>
-  <si>
-    <t>Units_System</t>
-  </si>
-  <si>
-    <t>SdcObsClassFK</t>
-  </si>
-  <si>
-    <t>ParentSpecimenFK</t>
-  </si>
-  <si>
-    <t>Datatype</t>
-  </si>
-  <si>
-    <t>SpecimenFK</t>
-  </si>
-  <si>
-    <t>PatientID</t>
-  </si>
-  <si>
-    <t>Response_Int</t>
-  </si>
-  <si>
-    <t>EncounterID</t>
-  </si>
-  <si>
-    <t>Response_Float</t>
-  </si>
-  <si>
-    <t>Response_DateTime</t>
-  </si>
-  <si>
-    <t>SpecimenTypeText</t>
-  </si>
-  <si>
-    <t>Reponse_String (nvarchar)</t>
-  </si>
-  <si>
-    <t>SpecimenTypeCode</t>
-  </si>
-  <si>
-    <t>ObsDateTime</t>
-  </si>
-  <si>
-    <t>SourceSiteText</t>
-  </si>
-  <si>
-    <t>SdcOrder</t>
-  </si>
-  <si>
-    <t>SourceSiteCode</t>
-  </si>
-  <si>
-    <t>SdcRepeatLevel</t>
-  </si>
-  <si>
-    <t>CollectionMethodText</t>
-  </si>
-  <si>
-    <t>SdcComments</t>
-  </si>
-  <si>
-    <t>CollectionMethodCode</t>
-  </si>
-  <si>
-    <t>SpecimenCount</t>
-  </si>
-  <si>
-    <t>CollectionDate</t>
+    <t>template_instance (DiagReport)</t>
+  </si>
+  <si>
+    <t>template_sdc</t>
+  </si>
+  <si>
+    <t>template_term_map</t>
+  </si>
+  <si>
+    <t>template_map_content</t>
+  </si>
+  <si>
+    <t>observation_specimens</t>
+  </si>
+  <si>
+    <t>doc_type (FD or Pkg)</t>
+  </si>
+  <si>
+    <t>template_instance_id</t>
+  </si>
+  <si>
+    <t>template_sdc_id</t>
+  </si>
+  <si>
+    <t>template_term_map_id</t>
+  </si>
+  <si>
+    <t>template_map_content_id</t>
+  </si>
+  <si>
+    <t>observation_specimens_id</t>
+  </si>
+  <si>
+    <t>person_id</t>
+  </si>
+  <si>
+    <t>parent_instance_guid</t>
+  </si>
+  <si>
+    <t>section_guid</t>
+  </si>
+  <si>
+    <t>list_item_text</t>
+  </si>
+  <si>
+    <t>list_item_instance_guid</t>
+  </si>
+  <si>
+    <t>list_item_parent_guid ?</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>units_system</t>
+  </si>
+  <si>
+    <t>response_int</t>
+  </si>
+  <si>
+    <t>response_float</t>
+  </si>
+  <si>
+    <t>response_datetime</t>
+  </si>
+  <si>
+    <t>response_string</t>
+  </si>
+  <si>
+    <t>obs_datetime</t>
+  </si>
+  <si>
+    <t>sdc_order</t>
+  </si>
+  <si>
+    <t>sdc_repeat_level</t>
+  </si>
+  <si>
+    <t>sdc_comments</t>
+  </si>
+  <si>
+    <t>template_instance_version_guid</t>
+  </si>
+  <si>
+    <t>template_instance_version_uri</t>
+  </si>
+  <si>
+    <t>instance_version_date</t>
+  </si>
+  <si>
+    <t>report_text</t>
+  </si>
+  <si>
+    <t>base_uri</t>
+  </si>
+  <si>
+    <t>lineage</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>full_uri</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>sdc_xml</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>map_xml</t>
+  </si>
+  <si>
+    <t>code_system_name</t>
+  </si>
+  <si>
+    <t>code_system_release_date</t>
+  </si>
+  <si>
+    <t>code_system_version</t>
+  </si>
+  <si>
+    <t>code_system_oid</t>
+  </si>
+  <si>
+    <t>code_system_uri</t>
+  </si>
+  <si>
+    <t>target_id</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>code_text</t>
+  </si>
+  <si>
+    <t>code_match</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>specimen_type_text</t>
+  </si>
+  <si>
+    <t>specimen_type_code</t>
+  </si>
+  <si>
+    <t>source_site_text</t>
+  </si>
+  <si>
+    <t>source_site_code</t>
+  </si>
+  <si>
+    <t>collection_method_text</t>
+  </si>
+  <si>
+    <t>collection_method_code</t>
+  </si>
+  <si>
+    <t>speciment_count</t>
+  </si>
+  <si>
+    <t>collection_date</t>
+  </si>
+  <si>
+    <t>section_sdcid</t>
+  </si>
+  <si>
+    <t>list_item_sdcid</t>
+  </si>
+  <si>
+    <t>surg_path_sdcid</t>
+  </si>
+  <si>
+    <t>template_map_sdcid</t>
+  </si>
+  <si>
+    <t>diag_report_props…</t>
+  </si>
+  <si>
+    <t>sdc_specimen</t>
+  </si>
+  <si>
+    <t>sdc_specimen_id</t>
+  </si>
+  <si>
+    <t>parent_sdc_specimen_id</t>
+  </si>
+  <si>
+    <t>sdc_observation</t>
+  </si>
+  <si>
+    <t>sdc_observation_id</t>
+  </si>
+  <si>
+    <t>parent_sdc_observation_id</t>
+  </si>
+  <si>
+    <t>sdc_form_design_sdcid (FD or Pkg)</t>
+  </si>
+  <si>
+    <t>visit_occurrence_id</t>
+  </si>
+  <si>
+    <t>provider_id</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>question_text</t>
+  </si>
+  <si>
+    <t>question_instance_guid</t>
+  </si>
+  <si>
+    <t>question_sdcid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1033,10 +1027,10 @@
       <xdr:rowOff>111125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2057400</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>13729</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>82378</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1056,8 +1050,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="831850" y="477838"/>
-          <a:ext cx="4073525" cy="3265487"/>
+          <a:off x="871194" y="323936"/>
+          <a:ext cx="4387292" cy="3513523"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1463,479 +1457,479 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77395545-5947-4993-9068-E6147EBA196F}">
   <dimension ref="B1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="29.1" thickBot="1">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="14.65" thickBot="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="45" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E4" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="15" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="46" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="46" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="25" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="2:6" ht="14.65" thickBot="1">
+    <row r="9" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="C9" s="6" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F9" s="28"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="2:6" ht="14.65" thickBot="1">
+    <row r="13" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="29"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="2:6" ht="14.65" thickBot="1">
+    <row r="15" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="14.65" thickBot="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="14.65" thickBot="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="30" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="14" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="41"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="14" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="14.65" thickBot="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="34" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="31" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D27" s="32"/>
       <c r="E27" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="14.65" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="31" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="31" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="35"/>
       <c r="E30" s="41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="14.65" thickBot="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="35"/>
       <c r="E31" s="42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="35"/>
       <c r="E32" s="38"/>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E33" s="38"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="E34" s="38"/>
       <c r="H34" s="38"/>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="35" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="H35" s="38"/>
     </row>
-    <row r="36" spans="2:8" ht="14.65" thickBot="1">
+    <row r="36" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
       <c r="H36" s="44"/>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H37" s="38"/>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H38" s="44"/>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H39" s="44"/>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H40" s="38"/>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H41" s="38"/>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H42" s="38"/>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H43" s="38"/>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H44" s="38"/>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H45" s="38"/>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H46" s="38"/>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H47" s="38"/>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H48" s="38"/>
     </row>
-    <row r="49" spans="8:8">
+    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H49" s="38"/>
     </row>
-    <row r="50" spans="8:8">
+    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H50" s="38"/>
     </row>
-    <row r="51" spans="8:8">
+    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H51" s="38"/>
     </row>
-    <row r="52" spans="8:8">
+    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H52" s="38"/>
     </row>
-    <row r="53" spans="8:8">
+    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H53" s="38"/>
     </row>
-    <row r="54" spans="8:8">
+    <row r="54" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H54" s="38"/>
     </row>
-    <row r="55" spans="8:8">
+    <row r="55" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H55" s="38"/>
     </row>
-    <row r="56" spans="8:8">
+    <row r="56" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H56" s="38"/>
     </row>
-    <row r="57" spans="8:8">
+    <row r="57" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H57" s="38"/>
     </row>
-    <row r="58" spans="8:8">
+    <row r="58" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H58" s="38"/>
     </row>
-    <row r="59" spans="8:8">
+    <row r="59" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H59" s="38"/>
     </row>
-    <row r="60" spans="8:8">
+    <row r="60" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H60" s="38"/>
     </row>
-    <row r="61" spans="8:8">
+    <row r="61" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H61" s="38"/>
     </row>
-    <row r="62" spans="8:8">
+    <row r="62" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H62" s="38"/>
     </row>
-    <row r="63" spans="8:8">
+    <row r="63" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H63" s="38"/>
     </row>
-    <row r="64" spans="8:8">
+    <row r="64" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H64" s="38"/>
     </row>
-    <row r="65" spans="8:8">
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H65" s="38"/>
     </row>
-    <row r="66" spans="8:8">
+    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H66" s="38"/>
     </row>
-    <row r="67" spans="8:8">
+    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H67" s="38"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update schema, update sdccdmlib
</commit_message>
<xml_diff>
--- a/database/SDC CDM Requirements.xlsx
+++ b/database/SDC CDM Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghavan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776214D8-9724-0144-A143-3DB2AAB18C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B56597-9E28-6041-A6C5-C9D06A19EEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="32000" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="31500" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="SdcObs" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>(other IDs etc.)</t>
   </si>
@@ -1458,7 +1458,7 @@
   <dimension ref="B1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1815,24 +1815,18 @@
       <c r="E32" s="38"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="35" t="s">
-        <v>13</v>
-      </c>
+      <c r="B33" s="35"/>
       <c r="E33" s="38"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="35" t="s">
-        <v>72</v>
-      </c>
+      <c r="B34" s="35"/>
       <c r="E34" s="38"/>
       <c r="H34" s="38"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="35" t="s">
-        <v>73</v>
-      </c>
+      <c r="B35" s="35"/>
       <c r="H35" s="38"/>
     </row>
     <row r="36" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add sdc template row data to schema, add row data csv, update library and notebook to import per-row data
</commit_message>
<xml_diff>
--- a/database/SDC CDM Requirements.xlsx
+++ b/database/SDC CDM Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghavan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776214D8-9724-0144-A143-3DB2AAB18C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B56597-9E28-6041-A6C5-C9D06A19EEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="32000" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="31500" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="SdcObs" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>(other IDs etc.)</t>
   </si>
@@ -1458,7 +1458,7 @@
   <dimension ref="B1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1815,24 +1815,18 @@
       <c r="E32" s="38"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="35" t="s">
-        <v>13</v>
-      </c>
+      <c r="B33" s="35"/>
       <c r="E33" s="38"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="35" t="s">
-        <v>72</v>
-      </c>
+      <c r="B34" s="35"/>
       <c r="E34" s="38"/>
       <c r="H34" s="38"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="35" t="s">
-        <v>73</v>
-      </c>
+      <c r="B35" s="35"/>
       <c r="H35" s="38"/>
     </row>
     <row r="36" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update spreadsheet: - add template_item table - mark any columns that reference OMOP tables
</commit_message>
<xml_diff>
--- a/database/SDC CDM Requirements.xlsx
+++ b/database/SDC CDM Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghavan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DCE2D5-9C4F-624A-831E-50DDF15E90C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1504CADB-07CF-9B43-A42E-0BFF222E23F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="31500" xr2:uid="{DE28B730-456E-4A19-85DD-0FCA7CBBA7BE}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
   <si>
     <t>(other IDs etc.)</t>
   </si>
@@ -120,9 +120,6 @@
     <t>observation_specimens_id</t>
   </si>
   <si>
-    <t>person_id</t>
-  </si>
-  <si>
     <t>parent_instance_guid</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>code_match</t>
   </si>
   <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>specimen_type_text</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>visit_occurrence_id</t>
   </si>
   <si>
-    <t>provider_id</t>
-  </si>
-  <si>
     <t>data_type</t>
   </si>
   <si>
@@ -346,13 +337,71 @@
   </si>
   <si>
     <t>max_cardinality</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">patient_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OMOP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">provider_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OMOP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">person_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OMOP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">visit_occurrence_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OMOP)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +536,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1204,7 +1259,7 @@
   <dimension ref="B1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1219,7 +1274,7 @@
   <sheetData>
     <row r="1" spans="2:7" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
@@ -1234,12 +1289,12 @@
         <v>5</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>8</v>
@@ -1254,7 +1309,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
@@ -1262,13 +1317,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>10</v>
@@ -1279,117 +1334,117 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="53" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="55" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -1398,68 +1453,68 @@
         <v>7</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="52" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
       <c r="G12" s="56" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="27"/>
       <c r="G13" s="41" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="14"/>
       <c r="G14" s="41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>1</v>
@@ -1467,12 +1522,12 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1481,121 +1536,121 @@
         <v>6</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D21" s="50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="37" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="37"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="34"/>
       <c r="D26" s="30"/>
       <c r="E26" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="32"/>
       <c r="D27" s="30"/>
       <c r="E27" s="37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="31"/>
       <c r="E28" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>